<commit_message>
hoja de depositos agregada
</commit_message>
<xml_diff>
--- a/Banco.xlsx
+++ b/Banco.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JUAN DAVID\Empresa\Negocio Cupos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Banco" sheetId="1" r:id="rId1"/>
+    <sheet name="Depositos" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Banco</t>
   </si>
@@ -54,16 +50,38 @@
   </si>
   <si>
     <t>TPS-957</t>
+  </si>
+  <si>
+    <t>DEPOSITOS</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Coopebombas</t>
+  </si>
+  <si>
+    <t>Reclamado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Titular </t>
+  </si>
+  <si>
+    <t>Gloria nancy lopez rios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +106,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -141,7 +166,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
@@ -153,6 +178,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -245,7 +279,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -280,7 +314,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -457,7 +491,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -468,7 +502,7 @@
   <dimension ref="A2:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +510,7 @@
     <col min="1" max="2" width="13.140625" style="6" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="5" max="5" width="17" style="6" customWidth="1"/>
     <col min="6" max="6" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -517,7 +551,7 @@
         <f>SUM(3447300+22000+60000)</f>
         <v>3529300</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -567,4 +601,80 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" style="6" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="40.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6">
+        <v>13</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="9">
+        <v>3447300</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
en depositos se agrego un estilo verde para la celda de cantidad
</commit_message>
<xml_diff>
--- a/Banco.xlsx
+++ b/Banco.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JUAN DAVID\Empresa\Negocio Cupos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Banco" sheetId="1" r:id="rId1"/>
     <sheet name="Depositos" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -79,9 +84,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,8 +123,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,6 +146,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -161,12 +179,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
@@ -183,14 +202,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="20% - Énfasis6" xfId="3" builtinId="50"/>
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,7 +508,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -501,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,22 +624,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" style="6" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" style="6" customWidth="1"/>
     <col min="3" max="3" width="26.5703125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" style="8" customWidth="1"/>
     <col min="5" max="5" width="26.7109375" style="6" customWidth="1"/>
     <col min="6" max="6" width="40.42578125" style="6" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="7" t="s">
         <v>10</v>
       </c>
@@ -632,7 +649,7 @@
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -653,7 +670,7 @@
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -663,7 +680,7 @@
       <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>3447300</v>
       </c>
       <c r="E6" s="6" t="s">

</xml_diff>